<commit_message>
finalized models and created color ramp for scelop CEWL heat map
</commit_message>
<xml_diff>
--- a/best models/all_exp_model_stats.xlsx
+++ b/best models/all_exp_model_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savannahweaver/Documents/github projects/Herpetology_2021/best models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C6B21D-7F45-D34C-9080-EF7EC27969EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93FA463-1D3C-9341-B359-850C8A0D284A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="18340" windowHeight="20180" xr2:uid="{99C447B3-75DF-974D-A3B1-B9AAA6CA7FDD}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="30080" windowHeight="20180" xr2:uid="{99C447B3-75DF-974D-A3B1-B9AAA6CA7FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
-  <si>
-    <t>(Intercept)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>CEWL ~</t>
   </si>
   <si>
-    <t>day:before</t>
-  </si>
-  <si>
-    <t>humidity treatment:dry</t>
-  </si>
-  <si>
-    <t>day * humidity treatment</t>
-  </si>
-  <si>
     <t>estimate</t>
   </si>
   <si>
@@ -81,19 +69,37 @@
     <t>&lt; 0.001</t>
   </si>
   <si>
-    <t>cloacal temperature</t>
-  </si>
-  <si>
-    <t>region:Ventrum</t>
-  </si>
-  <si>
-    <t>region:Head</t>
-  </si>
-  <si>
-    <t>region:Dewlap</t>
-  </si>
-  <si>
-    <t>region:Mite Patch</t>
+    <t>(intercept)</t>
+  </si>
+  <si>
+    <t>humidity treatment (dry)</t>
+  </si>
+  <si>
+    <t>region (ventrum)</t>
+  </si>
+  <si>
+    <t>region (head)</t>
+  </si>
+  <si>
+    <t>region (dewlap)</t>
+  </si>
+  <si>
+    <t>region (mite patch)</t>
+  </si>
+  <si>
+    <t>cloacal temperature at the time of measurement (℃)</t>
+  </si>
+  <si>
+    <t>day (after)</t>
+  </si>
+  <si>
+    <t>day (after) * humidity treatment (dry)</t>
+  </si>
+  <si>
+    <t>day * humidity treatment (dry)</t>
+  </si>
+  <si>
+    <t>&lt; 0.0001</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -143,6 +149,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +467,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,209 +480,209 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-51.112608431758403</v>
-      </c>
-      <c r="D3" s="2">
-        <v>10.969941924322301</v>
-      </c>
-      <c r="E3" s="2">
-        <v>-4.6593326367966403</v>
-      </c>
-      <c r="F3" s="2">
-        <v>220.89064885616099</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-69.375784903449699</v>
+      </c>
+      <c r="D3" s="4">
+        <v>11.8197221990293</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-5.8694936932736796</v>
+      </c>
+      <c r="F3" s="4">
+        <v>230.96964219851</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-18.26317646963</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.9250825011111601</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-9.4869578104255492</v>
-      </c>
-      <c r="F4" s="2">
-        <v>304.95405262659801</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="4">
+        <v>18.263176469806002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.9250825011117001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>9.4869578105142995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>304.95405323256699</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-19.377018041490899</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.8602792968802002</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-6.7745195592003897</v>
-      </c>
-      <c r="F5" s="2">
-        <v>44.796532319625697</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.76053159097103895</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.7927378035519199</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.27232473811317398</v>
+      </c>
+      <c r="F5" s="4">
+        <v>41.133118618782198</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.78673473866406696</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2">
-        <v>15.765056280988301</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.93957280798489</v>
-      </c>
-      <c r="E6" s="2">
-        <v>8.1281074967055709</v>
-      </c>
-      <c r="F6" s="2">
-        <v>286.00947770578301</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>15.7650562809789</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.9395728079888199</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8.1281074966842493</v>
+      </c>
+      <c r="F6" s="4">
+        <v>286.009477668572</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.9137684022003798</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.93957280798489</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.5022732790462401</v>
-      </c>
-      <c r="F7" s="2">
-        <v>286.00947769716203</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.134129807992943</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2.9137684021909802</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.9395728079888199</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.50227327903835</v>
+      </c>
+      <c r="F7" s="4">
+        <v>286.00947767441397</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.13412980799506699</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3.0976537768702102</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.9482735061326899</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.5899481089895999</v>
-      </c>
-      <c r="F8" s="2">
-        <v>286.09695221245403</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.112950888653805</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.0976537768641998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.9482735061366401</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.5899481089832901</v>
+      </c>
+      <c r="F8" s="4">
+        <v>286.09695220181101</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.11295088865526801</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3.7911890489459599</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.9564760504432901</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.9377640978978301</v>
-      </c>
-      <c r="F9" s="2">
-        <v>286.27000180966701</v>
-      </c>
-      <c r="G9" s="3">
-        <v>5.3635293484453499E-2</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.7911890489553799</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.95647605044726</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.9377640978987201</v>
+      </c>
+      <c r="F9" s="4">
+        <v>286.27000179867201</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5.3635293484382902E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3.8920479696034</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.48858126830253101</v>
-      </c>
-      <c r="E10" s="2">
-        <v>7.96601962069784</v>
-      </c>
-      <c r="F10" s="2">
-        <v>279.63436646644197</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3.8920479697064101</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.48858126829931797</v>
+      </c>
+      <c r="E10" s="4">
+        <v>7.9660196209610703</v>
+      </c>
+      <c r="F10" s="4">
+        <v>279.63437114745</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20.1375496328065</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2.4880774121298699</v>
-      </c>
-      <c r="E11" s="2">
-        <v>8.0936186047234493</v>
-      </c>
-      <c r="F11" s="2">
-        <v>288.342912181158</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="4">
+        <v>-20.1375496328845</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.48807741213446</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-8.0936186047398806</v>
+      </c>
+      <c r="F11" s="4">
+        <v>288.34291234635401</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -684,7 +691,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <v>10.883664551940001</v>
@@ -699,12 +706,12 @@
         <v>20.151932421188899</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <v>-0.12788470050742001</v>
@@ -719,12 +726,12 @@
         <v>110.92424110597599</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
         <v>-0.58887549318352805</v>
@@ -744,7 +751,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -753,7 +760,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <v>369.93790467850602</v>
@@ -768,12 +775,12 @@
         <v>4.1878194091273802</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C18" s="2">
         <v>-1.3147128062623901</v>
@@ -793,7 +800,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2">
         <v>-8.1518903809207899</v>
@@ -813,7 +820,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2">
         <v>1.90108196133484</v>
@@ -833,7 +840,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -842,7 +849,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2">
         <v>35.081015035857703</v>
@@ -857,12 +864,12 @@
         <v>4.5114860582386704</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C23" s="2">
         <v>-1.0534056460522101</v>
@@ -877,7 +884,7 @@
         <v>112.080897644169</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
redoing things without 2-day data and testing out figure options
</commit_message>
<xml_diff>
--- a/best models/all_exp_model_stats.xlsx
+++ b/best models/all_exp_model_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savannahweaver/Documents/github projects/Herpetology_2021/best models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93FA463-1D3C-9341-B359-850C8A0D284A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A1B05-0F73-3F46-900E-8C4C82CBE20F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="30080" windowHeight="20180" xr2:uid="{99C447B3-75DF-974D-A3B1-B9AAA6CA7FDD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>CEWL ~</t>
   </si>
@@ -48,9 +48,6 @@
     <t>t-value</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>osmolality ~</t>
   </si>
   <si>
@@ -96,10 +93,13 @@
     <t>day (after) * humidity treatment (dry)</t>
   </si>
   <si>
-    <t>day * humidity treatment (dry)</t>
-  </si>
-  <si>
     <t>&lt; 0.0001</t>
+  </si>
+  <si>
+    <t>day (mid)</t>
+  </si>
+  <si>
+    <t>day (mid) * humidity treatment (dry)</t>
   </si>
 </sst>
 </file>
@@ -464,18 +464,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D723C-7D89-DC4F-AAEF-B13C9CF4144B}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -489,10 +490,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -502,7 +503,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4">
         <v>-69.375784903449699</v>
@@ -517,12 +518,12 @@
         <v>230.96964219851</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4">
         <v>18.263176469806002</v>
@@ -537,12 +538,12 @@
         <v>304.95405323256699</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4">
         <v>0.76053159097103895</v>
@@ -562,7 +563,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>15.7650562809789</v>
@@ -577,12 +578,12 @@
         <v>286.009477668572</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4">
         <v>2.9137684021909802</v>
@@ -602,7 +603,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4">
         <v>3.0976537768641998</v>
@@ -622,7 +623,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4">
         <v>3.7911890489553799</v>
@@ -642,7 +643,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4">
         <v>3.8920479697064101</v>
@@ -657,12 +658,12 @@
         <v>279.63437114745</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4">
         <v>-20.1375496328845</v>
@@ -677,12 +678,12 @@
         <v>288.34291234635401</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -691,206 +692,288 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2">
-        <v>10.883664551940001</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.20373864696206001</v>
-      </c>
-      <c r="E13" s="2">
-        <v>53.419735107825403</v>
-      </c>
-      <c r="F13" s="2">
-        <v>20.151932421188899</v>
-      </c>
-      <c r="G13" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <v>10.3769451760934</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.22439268559085801</v>
+      </c>
+      <c r="E13" s="4">
+        <v>46.244578555532897</v>
+      </c>
+      <c r="F13" s="4">
+        <v>100.999999997624</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>-0.12788470050742001</v>
-      </c>
-      <c r="D14" s="2">
-        <v>3.2233326240839799E-2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>-3.9674683137537898</v>
-      </c>
-      <c r="F14" s="2">
-        <v>110.92424110597599</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-0.61728688527405395</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.27282504584974299</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-2.26257410990786</v>
+      </c>
+      <c r="F14" s="4">
+        <v>100.99999999777199</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2.5803006571743298E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2">
-        <v>-0.58887549318352805</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.20840935169157801</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-2.8255713498643602</v>
-      </c>
-      <c r="F15" s="2">
-        <v>111.108457541219</v>
-      </c>
-      <c r="G15" s="3">
-        <v>5.5971495530647702E-3</v>
+        <v>17</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-1.0308219364544899</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.27282504584974299</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-3.7783258983569001</v>
+      </c>
+      <c r="F15" s="4">
+        <v>100.99999999777199</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.45433159623644898</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.22285169557433099</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2.0387172512443801</v>
+      </c>
+      <c r="F16" s="4">
+        <v>100.999999998102</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4.40909258449107E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2">
-        <v>369.93790467850602</v>
-      </c>
-      <c r="D17" s="2">
-        <v>9.8039869175418897</v>
-      </c>
-      <c r="E17" s="2">
-        <v>37.733414761762901</v>
-      </c>
-      <c r="F17" s="2">
-        <v>4.1878194091273802</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2">
-        <v>-1.3147128062623901</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.87697444437640304</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-1.4991460865171</v>
-      </c>
-      <c r="F18" s="2">
-        <v>106.917358319616</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.136782698373699</v>
+        <v>10</v>
+      </c>
+      <c r="C18" s="4">
+        <v>368.294322927167</v>
+      </c>
+      <c r="D18" s="4">
+        <v>10.094991376666799</v>
+      </c>
+      <c r="E18" s="4">
+        <v>36.4828764270598</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4.4846729060523796</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1.01210420087086E-6</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="2">
-        <v>-8.1518903809207899</v>
-      </c>
-      <c r="D19" s="2">
-        <v>6.4385575778654101</v>
-      </c>
-      <c r="E19" s="2">
-        <v>-1.26610506815152</v>
-      </c>
-      <c r="F19" s="2">
-        <v>106.912297763038</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.20822730843909401</v>
+        <v>20</v>
+      </c>
+      <c r="C19" s="4">
+        <v>-17.176470588234899</v>
+      </c>
+      <c r="D19" s="4">
+        <v>6.8064122486609104</v>
+      </c>
+      <c r="E19" s="4">
+        <v>-2.5235718849698201</v>
+      </c>
+      <c r="F19" s="4">
+        <v>92.951110759141301</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1.33142302023167E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1.90108196133484</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1.2661121944720399</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1.5015114534360701</v>
-      </c>
-      <c r="F20" s="2">
-        <v>106.90817369349099</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.136171195715134</v>
+        <v>17</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3.8980579089779601</v>
+      </c>
+      <c r="D20" s="4">
+        <v>7.03862810875831</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.55380932885593503</v>
+      </c>
+      <c r="F20" s="4">
+        <v>92.971889700645505</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.58103887555425104</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>10.2149493910569</v>
+      </c>
+      <c r="D21" s="4">
+        <v>6.7131580975050102</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.52163098837987</v>
+      </c>
+      <c r="F21" s="4">
+        <v>92.955743227385597</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.13149614644426999</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2">
-        <v>35.081015035857703</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1.72782725393103</v>
-      </c>
-      <c r="E22" s="2">
-        <v>20.303543051565999</v>
-      </c>
-      <c r="F22" s="2">
-        <v>4.5114860582386704</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="4">
+        <v>-12.3235294117653</v>
+      </c>
+      <c r="D22" s="4">
+        <v>9.4910884209441502</v>
+      </c>
+      <c r="E22" s="4">
+        <v>-1.2984316303039301</v>
+      </c>
+      <c r="F22" s="4">
+        <v>92.951110761998905</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.19735132595211199</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2">
-        <v>-1.0534056460522101</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.180507479372014</v>
-      </c>
-      <c r="E23" s="2">
-        <v>-5.8358005425426596</v>
-      </c>
-      <c r="F23" s="2">
-        <v>112.080897644169</v>
-      </c>
-      <c r="G23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4">
+        <v>-17.783329455543502</v>
+      </c>
+      <c r="D23" s="4">
+        <v>9.7207971543447496</v>
+      </c>
+      <c r="E23" s="4">
+        <v>-1.82941061038344</v>
+      </c>
+      <c r="F23" s="4">
+        <v>92.954413140944595</v>
+      </c>
+      <c r="G23" s="4">
+        <v>7.0543972502939006E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C26" s="4">
+        <v>35.591574255057402</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1.7116680193613401</v>
+      </c>
+      <c r="E26" s="4">
+        <v>20.793503093162499</v>
+      </c>
+      <c r="F26" s="4">
+        <v>4.8534561623837096</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4">
+        <v>-5.7714285714285696</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.4722666473739801</v>
+      </c>
+      <c r="E27" s="4">
+        <v>-3.9200973422327001</v>
+      </c>
+      <c r="F27" s="4">
+        <v>98.766491740676102</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="4">
+        <v>-8.0571428571428498</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.4722666473739801</v>
+      </c>
+      <c r="E28" s="4">
+        <v>-5.4726111411367402</v>
+      </c>
+      <c r="F28" s="4">
+        <v>98.766491734250806</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>